<commit_message>
change in forti policy
</commit_message>
<xml_diff>
--- a/firewall_policies/Skybox_vLab_1.1.xlsx
+++ b/firewall_policies/Skybox_vLab_1.1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E5CA04-E380-4445-9FA2-8CC3FC0ED966}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD88C72-F61F-43BB-B2F2-809E11A3BDC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FortiBranch" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>Source</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>Internal DB</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>http,https,mysql</t>
+  </si>
+  <si>
+    <t>jb-m</t>
+  </si>
+  <si>
+    <t>jb-m1</t>
+  </si>
+  <si>
+    <t>w10-c</t>
+  </si>
+  <si>
+    <t>SSH</t>
   </si>
 </sst>
 </file>
@@ -396,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD0F028-4C1A-4F7C-8E95-263A98B92D2D}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,13 +449,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -445,10 +466,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -462,13 +483,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
@@ -479,35 +500,18 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -539,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>

</xml_diff>